<commit_message>
updated all SQL change MD files
</commit_message>
<xml_diff>
--- a/DIQ_Changes_Categories_Corrected.xlsx
+++ b/DIQ_Changes_Categories_Corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliascooper/Documents/GitHub/json_DIQs_Wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E88E6E-5885-6543-A0E1-52E8F3A63C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60CF943-B94B-064B-9536-C3EA964111AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deleted" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="363">
   <si>
     <t>UID</t>
   </si>
@@ -1135,6 +1135,9 @@
   </si>
   <si>
     <t>This was actually deleted</t>
+  </si>
+  <si>
+    <t>New? MD file not found</t>
   </si>
 </sst>
 </file>
@@ -1204,15 +1207,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1561,7 +1561,7 @@
       <c r="G1" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>353</v>
       </c>
     </row>
@@ -1954,13 +1954,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2094,14 +2094,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A63" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B76" sqref="A76:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="5"/>
+    <col min="4" max="4" width="8.83203125" style="4"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -2118,22 +2118,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2144,7 +2144,7 @@
       <c r="B2" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>279</v>
       </c>
       <c r="E2" t="s">
@@ -2167,7 +2167,7 @@
       <c r="B3" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>280</v>
       </c>
       <c r="E3" t="s">
@@ -2190,7 +2190,7 @@
       <c r="B4" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>281</v>
       </c>
       <c r="E4" t="s">
@@ -2213,7 +2213,7 @@
       <c r="B5" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>282</v>
       </c>
       <c r="E5" t="s">
@@ -2236,7 +2236,7 @@
       <c r="B6" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>283</v>
       </c>
       <c r="E6" t="s">
@@ -2259,7 +2259,7 @@
       <c r="B7" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>284</v>
       </c>
       <c r="E7" t="s">
@@ -2282,7 +2282,7 @@
       <c r="B8" t="s">
         <v>202</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>285</v>
       </c>
       <c r="E8" t="s">
@@ -2305,7 +2305,7 @@
       <c r="B9" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>286</v>
       </c>
       <c r="E9" t="s">
@@ -2328,7 +2328,7 @@
       <c r="B10" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>287</v>
       </c>
       <c r="E10" t="s">
@@ -2351,7 +2351,7 @@
       <c r="B11" t="s">
         <v>205</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>288</v>
       </c>
       <c r="E11" t="s">
@@ -2374,7 +2374,7 @@
       <c r="B12" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>289</v>
       </c>
       <c r="E12" t="s">
@@ -2400,7 +2400,7 @@
       <c r="B13" t="s">
         <v>207</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>290</v>
       </c>
       <c r="E13" t="s">
@@ -2423,7 +2423,7 @@
       <c r="B14" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>291</v>
       </c>
       <c r="E14" t="s">
@@ -2446,7 +2446,7 @@
       <c r="B15" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>292</v>
       </c>
       <c r="E15" t="s">
@@ -2469,7 +2469,7 @@
       <c r="B16" t="s">
         <v>210</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>293</v>
       </c>
       <c r="E16" t="s">
@@ -2492,7 +2492,7 @@
       <c r="B17" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>294</v>
       </c>
       <c r="E17" t="s">
@@ -2515,7 +2515,7 @@
       <c r="B18" t="s">
         <v>212</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>295</v>
       </c>
       <c r="E18" t="s">
@@ -2538,7 +2538,7 @@
       <c r="B19" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>296</v>
       </c>
       <c r="E19" t="s">
@@ -2561,7 +2561,7 @@
       <c r="B20" t="s">
         <v>214</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>297</v>
       </c>
       <c r="E20" t="s">
@@ -2584,7 +2584,7 @@
       <c r="B21" t="s">
         <v>215</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>298</v>
       </c>
       <c r="E21" t="s">
@@ -2607,7 +2607,7 @@
       <c r="B22" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>299</v>
       </c>
       <c r="E22" t="s">
@@ -2630,7 +2630,7 @@
       <c r="B23" t="s">
         <v>217</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>300</v>
       </c>
       <c r="E23" t="s">
@@ -2653,7 +2653,7 @@
       <c r="B24" t="s">
         <v>218</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>301</v>
       </c>
       <c r="E24" t="s">
@@ -2679,7 +2679,7 @@
       <c r="C25" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E25" t="s">
@@ -2702,7 +2702,7 @@
       <c r="B26" t="s">
         <v>219</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>302</v>
       </c>
       <c r="E26" t="s">
@@ -2725,7 +2725,7 @@
       <c r="B27" t="s">
         <v>220</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>303</v>
       </c>
       <c r="E27" t="s">
@@ -2748,7 +2748,7 @@
       <c r="B28" t="s">
         <v>221</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>304</v>
       </c>
       <c r="E28" t="s">
@@ -2771,7 +2771,7 @@
       <c r="B29" t="s">
         <v>222</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>305</v>
       </c>
       <c r="E29" t="s">
@@ -2794,7 +2794,7 @@
       <c r="B30" t="s">
         <v>223</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>306</v>
       </c>
       <c r="E30" t="s">
@@ -2817,7 +2817,7 @@
       <c r="B31" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>307</v>
       </c>
       <c r="E31" t="s">
@@ -2840,7 +2840,7 @@
       <c r="B32" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>308</v>
       </c>
       <c r="E32" t="s">
@@ -2863,7 +2863,7 @@
       <c r="B33" t="s">
         <v>226</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>307</v>
       </c>
       <c r="E33" t="s">
@@ -2886,7 +2886,7 @@
       <c r="B34" t="s">
         <v>227</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>309</v>
       </c>
       <c r="E34" t="s">
@@ -2909,7 +2909,7 @@
       <c r="B35" t="s">
         <v>228</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>310</v>
       </c>
       <c r="E35" t="s">
@@ -2932,7 +2932,7 @@
       <c r="B36" t="s">
         <v>229</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>311</v>
       </c>
       <c r="E36" t="s">
@@ -2955,7 +2955,7 @@
       <c r="B37" t="s">
         <v>230</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>312</v>
       </c>
       <c r="E37" t="s">
@@ -2978,7 +2978,7 @@
       <c r="B38" t="s">
         <v>231</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>313</v>
       </c>
       <c r="E38" t="s">
@@ -3001,7 +3001,7 @@
       <c r="B39" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>314</v>
       </c>
       <c r="E39" t="s">
@@ -3024,7 +3024,7 @@
       <c r="B40" t="s">
         <v>233</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>313</v>
       </c>
       <c r="E40" t="s">
@@ -3047,7 +3047,7 @@
       <c r="B41" t="s">
         <v>234</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>315</v>
       </c>
       <c r="E41" t="s">
@@ -3070,7 +3070,7 @@
       <c r="B42" t="s">
         <v>235</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>316</v>
       </c>
       <c r="E42" t="s">
@@ -3093,8 +3093,20 @@
       <c r="B43" t="s">
         <v>236</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>317</v>
+      </c>
+      <c r="E43" t="s">
+        <v>348</v>
+      </c>
+      <c r="F43" t="s">
+        <v>348</v>
+      </c>
+      <c r="G43" t="s">
+        <v>348</v>
+      </c>
+      <c r="H43" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3104,8 +3116,20 @@
       <c r="B44" t="s">
         <v>237</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>318</v>
+      </c>
+      <c r="E44" t="s">
+        <v>348</v>
+      </c>
+      <c r="F44" t="s">
+        <v>348</v>
+      </c>
+      <c r="G44" t="s">
+        <v>348</v>
+      </c>
+      <c r="H44" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -3115,8 +3139,20 @@
       <c r="B45" t="s">
         <v>238</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>319</v>
+      </c>
+      <c r="E45" t="s">
+        <v>348</v>
+      </c>
+      <c r="F45" t="s">
+        <v>348</v>
+      </c>
+      <c r="G45" t="s">
+        <v>348</v>
+      </c>
+      <c r="H45" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -3126,8 +3162,20 @@
       <c r="B46" t="s">
         <v>239</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>320</v>
+      </c>
+      <c r="E46" t="s">
+        <v>348</v>
+      </c>
+      <c r="F46" t="s">
+        <v>348</v>
+      </c>
+      <c r="G46" t="s">
+        <v>348</v>
+      </c>
+      <c r="H46" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -3137,8 +3185,20 @@
       <c r="B47" t="s">
         <v>240</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>321</v>
+      </c>
+      <c r="E47" t="s">
+        <v>348</v>
+      </c>
+      <c r="F47" t="s">
+        <v>348</v>
+      </c>
+      <c r="G47" t="s">
+        <v>348</v>
+      </c>
+      <c r="H47" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -3148,415 +3208,862 @@
       <c r="B48" t="s">
         <v>241</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>348</v>
+      </c>
+      <c r="F48" t="s">
+        <v>348</v>
+      </c>
+      <c r="G48" t="s">
+        <v>348</v>
+      </c>
+      <c r="H48" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>159</v>
       </c>
       <c r="B49" t="s">
         <v>242</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>348</v>
+      </c>
+      <c r="F49" t="s">
+        <v>348</v>
+      </c>
+      <c r="G49" t="s">
+        <v>348</v>
+      </c>
+      <c r="H49" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>160</v>
       </c>
       <c r="B50" t="s">
         <v>243</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>348</v>
+      </c>
+      <c r="F50" t="s">
+        <v>348</v>
+      </c>
+      <c r="G50" t="s">
+        <v>348</v>
+      </c>
+      <c r="H50" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>161</v>
       </c>
       <c r="B51" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="4" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>348</v>
+      </c>
+      <c r="F51" t="s">
+        <v>348</v>
+      </c>
+      <c r="G51" t="s">
+        <v>348</v>
+      </c>
+      <c r="H51" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>162</v>
       </c>
       <c r="B52" t="s">
         <v>245</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>348</v>
+      </c>
+      <c r="F52" t="s">
+        <v>348</v>
+      </c>
+      <c r="G52" t="s">
+        <v>348</v>
+      </c>
+      <c r="H52" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>163</v>
       </c>
       <c r="B53" t="s">
         <v>246</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="4" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>348</v>
+      </c>
+      <c r="F53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H53" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>164</v>
       </c>
       <c r="B54" t="s">
         <v>247</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>348</v>
+      </c>
+      <c r="F54" t="s">
+        <v>348</v>
+      </c>
+      <c r="G54" t="s">
+        <v>348</v>
+      </c>
+      <c r="H54" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>165</v>
       </c>
       <c r="B55" t="s">
         <v>248</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>348</v>
+      </c>
+      <c r="F55" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" t="s">
+        <v>348</v>
+      </c>
+      <c r="H55" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>166</v>
       </c>
       <c r="B56" t="s">
         <v>249</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>348</v>
+      </c>
+      <c r="F56" t="s">
+        <v>348</v>
+      </c>
+      <c r="G56" t="s">
+        <v>348</v>
+      </c>
+      <c r="H56" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>167</v>
       </c>
       <c r="B57" t="s">
         <v>250</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>348</v>
+      </c>
+      <c r="F57" t="s">
+        <v>348</v>
+      </c>
+      <c r="G57" t="s">
+        <v>348</v>
+      </c>
+      <c r="H57" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>168</v>
       </c>
       <c r="B58" t="s">
         <v>251</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>348</v>
+      </c>
+      <c r="F58" t="s">
+        <v>348</v>
+      </c>
+      <c r="G58" t="s">
+        <v>348</v>
+      </c>
+      <c r="H58" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>169</v>
       </c>
       <c r="B59" t="s">
         <v>252</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>348</v>
+      </c>
+      <c r="F59" t="s">
+        <v>348</v>
+      </c>
+      <c r="G59" t="s">
+        <v>348</v>
+      </c>
+      <c r="H59" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>170</v>
       </c>
       <c r="B60" t="s">
         <v>253</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>348</v>
+      </c>
+      <c r="F60" t="s">
+        <v>348</v>
+      </c>
+      <c r="G60" t="s">
+        <v>348</v>
+      </c>
+      <c r="H60" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>171</v>
       </c>
       <c r="B61" t="s">
         <v>254</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>348</v>
+      </c>
+      <c r="F61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G61" t="s">
+        <v>348</v>
+      </c>
+      <c r="H61" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>172</v>
       </c>
       <c r="B62" t="s">
         <v>255</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>348</v>
+      </c>
+      <c r="F62" t="s">
+        <v>348</v>
+      </c>
+      <c r="G62" t="s">
+        <v>348</v>
+      </c>
+      <c r="H62" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>173</v>
       </c>
       <c r="B63" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>348</v>
+      </c>
+      <c r="F63" t="s">
+        <v>348</v>
+      </c>
+      <c r="G63" t="s">
+        <v>348</v>
+      </c>
+      <c r="H63" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>174</v>
       </c>
       <c r="B64" t="s">
         <v>257</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>348</v>
+      </c>
+      <c r="F64" t="s">
+        <v>348</v>
+      </c>
+      <c r="G64" t="s">
+        <v>348</v>
+      </c>
+      <c r="H64" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>175</v>
       </c>
       <c r="B65" t="s">
         <v>258</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>348</v>
+      </c>
+      <c r="F65" t="s">
+        <v>348</v>
+      </c>
+      <c r="G65" t="s">
+        <v>348</v>
+      </c>
+      <c r="H65" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>176</v>
       </c>
       <c r="B66" t="s">
         <v>259</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>348</v>
+      </c>
+      <c r="F66" t="s">
+        <v>348</v>
+      </c>
+      <c r="G66" t="s">
+        <v>348</v>
+      </c>
+      <c r="H66" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>177</v>
       </c>
       <c r="B67" t="s">
         <v>260</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>348</v>
+      </c>
+      <c r="F67" t="s">
+        <v>348</v>
+      </c>
+      <c r="G67" t="s">
+        <v>348</v>
+      </c>
+      <c r="H67" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>178</v>
       </c>
       <c r="B68" t="s">
         <v>261</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="4" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>348</v>
+      </c>
+      <c r="F68" t="s">
+        <v>348</v>
+      </c>
+      <c r="G68" t="s">
+        <v>348</v>
+      </c>
+      <c r="H68" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>179</v>
       </c>
       <c r="B69" t="s">
         <v>262</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>348</v>
+      </c>
+      <c r="F69" t="s">
+        <v>348</v>
+      </c>
+      <c r="G69" t="s">
+        <v>348</v>
+      </c>
+      <c r="H69" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>180</v>
       </c>
       <c r="B70" t="s">
         <v>263</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="4" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>348</v>
+      </c>
+      <c r="F70" t="s">
+        <v>348</v>
+      </c>
+      <c r="G70" t="s">
+        <v>348</v>
+      </c>
+      <c r="H70" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>181</v>
       </c>
       <c r="B71" t="s">
         <v>264</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="4" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>348</v>
+      </c>
+      <c r="F71" t="s">
+        <v>348</v>
+      </c>
+      <c r="G71" t="s">
+        <v>348</v>
+      </c>
+      <c r="H71" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>182</v>
       </c>
       <c r="B72" t="s">
         <v>265</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>348</v>
+      </c>
+      <c r="F72" t="s">
+        <v>348</v>
+      </c>
+      <c r="G72" t="s">
+        <v>348</v>
+      </c>
+      <c r="H72" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>183</v>
       </c>
       <c r="B73" t="s">
         <v>266</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="4" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>348</v>
+      </c>
+      <c r="F73" t="s">
+        <v>348</v>
+      </c>
+      <c r="G73" t="s">
+        <v>348</v>
+      </c>
+      <c r="H73" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>184</v>
       </c>
       <c r="B74" t="s">
         <v>267</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="4" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>348</v>
+      </c>
+      <c r="F74" t="s">
+        <v>348</v>
+      </c>
+      <c r="G74" t="s">
+        <v>348</v>
+      </c>
+      <c r="H74" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>185</v>
       </c>
       <c r="B75" t="s">
         <v>268</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="4" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>348</v>
+      </c>
+      <c r="F75" t="s">
+        <v>348</v>
+      </c>
+      <c r="G75" t="s">
+        <v>348</v>
+      </c>
+      <c r="H75" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>186</v>
       </c>
       <c r="B76" t="s">
         <v>269</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>187</v>
       </c>
       <c r="B77" t="s">
         <v>270</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>348</v>
+      </c>
+      <c r="F77" t="s">
+        <v>348</v>
+      </c>
+      <c r="G77" t="s">
+        <v>348</v>
+      </c>
+      <c r="H77" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>188</v>
       </c>
       <c r="B78" t="s">
         <v>271</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>348</v>
+      </c>
+      <c r="F78" t="s">
+        <v>348</v>
+      </c>
+      <c r="G78" t="s">
+        <v>348</v>
+      </c>
+      <c r="H78" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>189</v>
       </c>
       <c r="B79" t="s">
         <v>272</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>348</v>
+      </c>
+      <c r="F79" t="s">
+        <v>348</v>
+      </c>
+      <c r="G79" t="s">
+        <v>348</v>
+      </c>
+      <c r="H79" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>190</v>
       </c>
       <c r="B80" t="s">
         <v>273</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="4" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>348</v>
+      </c>
+      <c r="F80" t="s">
+        <v>348</v>
+      </c>
+      <c r="G80" t="s">
+        <v>348</v>
+      </c>
+      <c r="H80" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>191</v>
       </c>
       <c r="B81" t="s">
         <v>274</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="4" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>348</v>
+      </c>
+      <c r="F81" t="s">
+        <v>348</v>
+      </c>
+      <c r="G81" t="s">
+        <v>348</v>
+      </c>
+      <c r="H81" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>192</v>
       </c>
       <c r="B82" t="s">
         <v>275</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>348</v>
+      </c>
+      <c r="F82" t="s">
+        <v>348</v>
+      </c>
+      <c r="G82" t="s">
+        <v>348</v>
+      </c>
+      <c r="H82" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>193</v>
       </c>
       <c r="B83" t="s">
         <v>276</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="4" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>348</v>
+      </c>
+      <c r="F83" t="s">
+        <v>348</v>
+      </c>
+      <c r="G83" t="s">
+        <v>348</v>
+      </c>
+      <c r="H83" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>194</v>
       </c>
       <c r="B84" t="s">
         <v>277</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="s">
+        <v>348</v>
+      </c>
+      <c r="F84" t="s">
+        <v>348</v>
+      </c>
+      <c r="G84" t="s">
+        <v>348</v>
+      </c>
+      <c r="H84" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>195</v>
       </c>
       <c r="B85" t="s">
         <v>278</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="4" t="s">
         <v>343</v>
+      </c>
+      <c r="E85" t="s">
+        <v>348</v>
+      </c>
+      <c r="F85" t="s">
+        <v>348</v>
+      </c>
+      <c r="G85" t="s">
+        <v>348</v>
+      </c>
+      <c r="H85" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3567,10 +4074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3795,6 +4302,14 @@
       </c>
       <c r="B27" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final changes: updated MDs for DIQs whose scripts were truncated
</commit_message>
<xml_diff>
--- a/DIQ_Changes_Categories_Corrected.xlsx
+++ b/DIQ_Changes_Categories_Corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliascooper/Documents/GitHub/json_DIQs_Wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57DDE8E-F59F-6A42-9B50-B6D9354C8B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC9F77-69DC-9B4C-A069-EE5C9C031570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deleted" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="325">
   <si>
     <t>UID</t>
   </si>
@@ -1017,13 +1017,13 @@
     <t>This was actually deleted</t>
   </si>
   <si>
-    <t>New? MD file not found</t>
-  </si>
-  <si>
     <t>Deleted before MD creation</t>
   </si>
   <si>
     <t>MD Created?</t>
+  </si>
+  <si>
+    <t>DELETED</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1106,10 +1106,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1418,7 +1414,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1456,7 +1452,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>9030092</v>
       </c>
       <c r="B2" t="s">
@@ -1479,7 +1475,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>1030093</v>
       </c>
       <c r="B3" t="s">
@@ -1502,7 +1498,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4">
         <v>9030094</v>
       </c>
       <c r="B4" t="s">
@@ -1525,7 +1521,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5">
         <v>1030110</v>
       </c>
       <c r="B5" t="s">
@@ -1548,7 +1544,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6">
         <v>9060285</v>
       </c>
       <c r="B6" t="s">
@@ -1574,7 +1570,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7">
         <v>9060289</v>
       </c>
       <c r="B7" t="s">
@@ -1600,7 +1596,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8">
         <v>9060288</v>
       </c>
       <c r="B8" t="s">
@@ -1623,7 +1619,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9">
         <v>9080395</v>
       </c>
       <c r="B9" t="s">
@@ -1646,7 +1642,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10">
         <v>9060286</v>
       </c>
       <c r="B10" t="s">
@@ -1669,7 +1665,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>9010024</v>
       </c>
       <c r="B11" t="s">
@@ -1692,7 +1688,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12">
         <v>1060241</v>
       </c>
       <c r="B12" t="s">
@@ -1718,7 +1714,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>1060240</v>
       </c>
       <c r="B13" t="s">
@@ -1741,7 +1737,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>9080421</v>
       </c>
       <c r="B14" t="s">
@@ -1764,7 +1760,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>9080422</v>
       </c>
       <c r="B15" t="s">
@@ -1787,7 +1783,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16">
         <v>9030068</v>
       </c>
       <c r="B16" t="s">
@@ -1813,14 +1809,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>9050283</v>
       </c>
       <c r="B17" t="s">
         <v>229</v>
       </c>
       <c r="C17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E17" t="s">
         <v>312</v>
@@ -1836,14 +1832,14 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18">
         <v>1030111</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E18" t="s">
         <v>312</v>
@@ -1859,14 +1855,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>9080434</v>
       </c>
       <c r="B19" t="s">
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E19" t="s">
         <v>312</v>
@@ -2053,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B76" sqref="A76:B76"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3815,7 +3811,7 @@
         <v>267</v>
       </c>
       <c r="I76" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4033,9 +4029,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
@@ -4054,12 +4050,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>324</v>
+      <c r="E1" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>9060304</v>
       </c>
       <c r="B2" t="s">
@@ -4070,7 +4066,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>9060305</v>
       </c>
       <c r="B3" t="s">
@@ -4081,7 +4077,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4">
         <v>1030113</v>
       </c>
       <c r="B4" t="s">
@@ -4092,7 +4088,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5">
         <v>1030117</v>
       </c>
       <c r="B5" t="s">
@@ -4103,7 +4099,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6">
         <v>9060306</v>
       </c>
       <c r="B6" t="s">
@@ -4114,7 +4110,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7">
         <v>9060307</v>
       </c>
       <c r="B7" t="s">
@@ -4125,7 +4121,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8">
         <v>9080411</v>
       </c>
       <c r="B8" t="s">
@@ -4136,7 +4132,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9">
         <v>1060269</v>
       </c>
       <c r="B9" t="s">
@@ -4147,7 +4143,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10">
         <v>1030094</v>
       </c>
       <c r="B10" t="s">
@@ -4158,7 +4154,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>1030095</v>
       </c>
       <c r="B11" t="s">
@@ -4169,7 +4165,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12">
         <v>1030112</v>
       </c>
       <c r="B12" t="s">
@@ -4180,7 +4176,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>1030098</v>
       </c>
       <c r="B13" t="s">
@@ -4191,7 +4187,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>9080433</v>
       </c>
       <c r="B14" t="s">
@@ -4202,7 +4198,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>9080410</v>
       </c>
       <c r="B15" t="s">
@@ -4213,7 +4209,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16">
         <v>9060302</v>
       </c>
       <c r="B16" t="s">
@@ -4224,7 +4220,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>9060303</v>
       </c>
       <c r="B17" t="s">
@@ -4235,7 +4231,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18">
         <v>1060262</v>
       </c>
       <c r="B18" t="s">
@@ -4246,7 +4242,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>1060264</v>
       </c>
       <c r="B19" t="s">
@@ -4257,7 +4253,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="A20">
         <v>1060265</v>
       </c>
       <c r="B20" t="s">
@@ -4268,7 +4264,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21">
         <v>1060266</v>
       </c>
       <c r="B21" t="s">
@@ -4279,7 +4275,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22">
         <v>1060267</v>
       </c>
       <c r="B22" t="s">
@@ -4290,7 +4286,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
+      <c r="A23">
         <v>1030114</v>
       </c>
       <c r="B23" t="s">
@@ -4301,7 +4297,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
+      <c r="A24">
         <v>1030115</v>
       </c>
       <c r="B24" t="s">
@@ -4312,7 +4308,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
+      <c r="A25">
         <v>1030116</v>
       </c>
       <c r="B25" t="s">
@@ -4321,9 +4317,6 @@
       <c r="E25" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4332,15 +4325,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6473289-A163-1A47-8E06-6D7DC1188232}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4353,8 +4346,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -4364,8 +4360,11 @@
       <c r="D2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -4375,8 +4374,11 @@
       <c r="D3" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -4386,8 +4388,11 @@
       <c r="D4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -4397,8 +4402,11 @@
       <c r="D5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -4408,8 +4416,11 @@
       <c r="D6" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -4419,8 +4430,11 @@
       <c r="D7" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -4430,8 +4444,11 @@
       <c r="D8" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4441,8 +4458,11 @@
       <c r="D9" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -4451,6 +4471,9 @@
       </c>
       <c r="D10" t="s">
         <v>306</v>
+      </c>
+      <c r="E10" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final pass w minor clean up
</commit_message>
<xml_diff>
--- a/DIQ_Changes_Categories_Corrected.xlsx
+++ b/DIQ_Changes_Categories_Corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliascooper/Documents/GitHub/json_DIQs_Wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC9F77-69DC-9B4C-A069-EE5C9C031570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C40C49-75B3-1C47-8E5F-7F6041A28144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deleted" sheetId="1" r:id="rId1"/>
@@ -2049,7 +2049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
@@ -4032,10 +4032,13 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="B25" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -4327,11 +4330,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6473289-A163-1A47-8E06-6D7DC1188232}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>